<commit_message>
Unhide columns and convert spreadsheets to .xlsx
</commit_message>
<xml_diff>
--- a/requirements/CAP.xlsx
+++ b/requirements/CAP.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sfaily/webinos/webinos-design-data/requirements/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35460" yWindow="165" windowWidth="24240" windowHeight="8520" tabRatio="500"/>
+    <workbookView xWindow="3560" yWindow="500" windowWidth="39400" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="In scope" sheetId="1" r:id="rId1"/>
     <sheet name="Out of scope" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -746,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -757,11 +765,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1099,1014 +1121,1014 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22:O22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="1"/>
-    <col min="5" max="5" width="66.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="30" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="10.875" style="1"/>
-    <col min="13" max="14" width="22.875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="31" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="6"/>
+    <col min="5" max="5" width="66.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="30" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" style="6" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" style="6"/>
+    <col min="13" max="14" width="22.83203125" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="O2" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="O2" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M3" s="5" t="s">
+      <c r="K3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M4" s="5" t="s">
+      <c r="I4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="O4" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="O4" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="I5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5" t="s">
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="O5" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="O5" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="I6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5" t="s">
+      <c r="K6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="O6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="O6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="I7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5" t="s">
+      <c r="K7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="O7" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="O7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="I8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5" t="s">
+      <c r="K8" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="O8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5" t="s">
+      <c r="I9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="5" t="s">
+      <c r="I10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="K10" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5" t="s">
+      <c r="I11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="O11" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="O11" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="I12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5" t="s">
+      <c r="K12" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="O12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="O12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="F13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5" t="s">
+      <c r="I13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="O13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="O13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="5" t="s">
+      <c r="I14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5" t="s">
+      <c r="K14" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="C15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="F15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="I15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5" t="s">
+      <c r="K15" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="O15" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="O15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="F16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16" s="5" t="s">
+      <c r="I16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5" t="s">
+      <c r="K16" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="O16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="O16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="C17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="F17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="I17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5" t="s">
+      <c r="K17" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="O17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="347.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="O17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="353" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="C18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="F18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="I18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5" t="s">
+      <c r="K18" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="O18" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="O18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="F19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="I19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5" t="s">
+      <c r="K19" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="O19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="O19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="C20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="5" t="s">
+      <c r="I20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="K20" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5" t="s">
+      <c r="K20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="O20" s="5" t="s">
+      <c r="O20" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="C21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="F21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J21" s="5" t="s">
+      <c r="I21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K21" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5" t="s">
+      <c r="K21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="O21" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:15" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="I22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="K22" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5" t="s">
+      <c r="K22" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="O22" s="5">
+      <c r="O22" s="8">
         <v>1</v>
       </c>
     </row>
@@ -2116,38 +2138,33 @@
     <sortCondition ref="A1:A41"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="1"/>
-    <col min="5" max="5" width="66.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="66.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="30" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.875" style="1"/>
-    <col min="9" max="9" width="17.625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.875" style="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="17.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>145</v>
       </c>
@@ -2176,7 +2193,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>129</v>
       </c>
@@ -2205,7 +2222,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -2234,7 +2251,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>109</v>
       </c>
@@ -2263,7 +2280,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>93</v>
       </c>
@@ -2292,7 +2309,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -2321,7 +2338,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
@@ -2350,7 +2367,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>84</v>
       </c>
@@ -2379,7 +2396,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>88</v>
       </c>
@@ -2408,7 +2425,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
@@ -2437,7 +2454,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>103</v>
       </c>
@@ -2466,7 +2483,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>106</v>
       </c>
@@ -2495,7 +2512,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -2524,7 +2541,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>75</v>
       </c>
@@ -2553,7 +2570,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>96</v>
       </c>
@@ -2582,7 +2599,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>100</v>
       </c>
@@ -2611,7 +2628,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
@@ -2640,7 +2657,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -2669,7 +2686,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -2698,7 +2715,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -2727,7 +2744,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>91</v>
       </c>
@@ -2758,10 +2775,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>